<commit_message>
added wine dataset with gradually increasing number of relevant attributes
</commit_message>
<xml_diff>
--- a/proj1/report/data.xlsx
+++ b/proj1/report/data.xlsx
@@ -17,6 +17,7 @@
   <definedNames>
     <definedName name="our_accuracy" localSheetId="0">Sheet1!$A$3:$K$7</definedName>
     <definedName name="our_accuracy_animals" localSheetId="0">Sheet1!$M$3:$W$7</definedName>
+    <definedName name="our_accuracy_wine_2_relevant_1" localSheetId="0">Sheet1!$AA$5:$AK$8</definedName>
     <definedName name="scikit_accuracy" localSheetId="0">Sheet1!$A$10:$K$15</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -67,7 +68,24 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="scikit_accuracy" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="our_accuracy-wine-2-relevant" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" firstRow="3" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/our_accuracy-wine-2-relevant.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="scikit_accuracy" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Jerry/Documents/thick-filling/proj1/code/scikit_accuracy.csv" tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -88,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>IRIS DATASET PERFORMANCE</t>
   </si>
@@ -104,12 +122,24 @@
   <si>
     <t>K-NN</t>
   </si>
+  <si>
+    <t>WINE DATASET PERFORMANCE</t>
+  </si>
+  <si>
+    <t>Average Accuracy on Changing Number of Relevant Attributes (3-NN)</t>
+  </si>
+  <si>
+    <t>Number of Relevant Attributes</t>
+  </si>
+  <si>
+    <t>Average Accuracy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +158,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,22 +202,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -679,11 +730,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1979980992"/>
-        <c:axId val="1936891360"/>
+        <c:axId val="-1108098976"/>
+        <c:axId val="-1150582464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1979980992"/>
+        <c:axId val="-1108098976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -795,12 +846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1936891360"/>
+        <c:crossAx val="-1150582464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1936891360"/>
+        <c:axId val="-1150582464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -912,7 +963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1979980992"/>
+        <c:crossAx val="-1108098976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1280,11 +1331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1895543392"/>
-        <c:axId val="1895547424"/>
+        <c:axId val="-1072612144"/>
+        <c:axId val="-1072608752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1895543392"/>
+        <c:axId val="-1072612144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -1389,12 +1440,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1895547424"/>
+        <c:crossAx val="-1072608752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1895547424"/>
+        <c:axId val="-1072608752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1506,7 +1557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1895543392"/>
+        <c:crossAx val="-1072612144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1869,11 +1920,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1980004976"/>
-        <c:axId val="1980008736"/>
+        <c:axId val="-1072577840"/>
+        <c:axId val="-1072573808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1980004976"/>
+        <c:axId val="-1072577840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -1978,12 +2029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980008736"/>
+        <c:crossAx val="-1072573808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1980008736"/>
+        <c:axId val="-1072573808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2096,7 +2147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980004976"/>
+        <c:crossAx val="-1072577840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2458,11 +2509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1980035920"/>
-        <c:axId val="1980039952"/>
+        <c:axId val="-1072547232"/>
+        <c:axId val="-1072543200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1980035920"/>
+        <c:axId val="-1072547232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -2566,12 +2617,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980039952"/>
+        <c:crossAx val="-1072543200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1980039952"/>
+        <c:axId val="-1072543200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2684,7 +2735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980035920"/>
+        <c:crossAx val="-1072547232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3045,11 +3096,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1936905312"/>
-        <c:axId val="1936908704"/>
+        <c:axId val="-1072525296"/>
+        <c:axId val="-1072521264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1936905312"/>
+        <c:axId val="-1072525296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -3161,12 +3212,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1936908704"/>
+        <c:crossAx val="-1072521264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1936908704"/>
+        <c:axId val="-1072521264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3278,7 +3329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1936905312"/>
+        <c:crossAx val="-1072525296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3656,11 +3707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2015114656"/>
-        <c:axId val="2058597424"/>
+        <c:axId val="-1072491856"/>
+        <c:axId val="-1072487824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2015114656"/>
+        <c:axId val="-1072491856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -3765,12 +3816,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2058597424"/>
+        <c:crossAx val="-1072487824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2058597424"/>
+        <c:axId val="-1072487824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3882,7 +3933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2015114656"/>
+        <c:crossAx val="-1072491856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4444,11 +4495,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2055713584"/>
-        <c:axId val="2018830992"/>
+        <c:axId val="-1108054320"/>
+        <c:axId val="-1108049776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2055713584"/>
+        <c:axId val="-1108054320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -4560,12 +4611,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2018830992"/>
+        <c:crossAx val="-1108049776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2018830992"/>
+        <c:axId val="-1108049776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -4677,7 +4728,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2055713584"/>
+        <c:crossAx val="-1108054320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4754,6 +4805,460 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Accuracy on Changing Number of Relevant Attributes (3-NN)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$5:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$5:$Z$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>78.16743829724631</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.10190845516119</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.2230602387463</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.3872378120288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.9412467154564</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.0806595846384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1013327136"/>
+        <c:axId val="-1014940752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1013327136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Relevant</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Attributes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1014940752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1014940752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1013327136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4899,6 +5404,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -8492,6 +9037,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8731,11 +9792,41 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>489185</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>110066</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>82314</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82314</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scikit_accuracy" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy-wine-2-relevant_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8743,6 +9834,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scikit_accuracy" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -9009,10 +10104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9021,66 +10116,99 @@
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="13" max="22" width="13" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.5" customWidth="1"/>
+    <col min="25" max="25" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="34" width="13" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13" customWidth="1"/>
+    <col min="36" max="36" width="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -9148,8 +10276,22 @@
       <c r="W3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>95.564177952547396</v>
       </c>
@@ -9184,41 +10326,48 @@
         <v>1</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="5">
+      <c r="M4" s="3">
         <v>89.860501319999997</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="3">
         <v>82.655543199999997</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="3">
         <v>61.226753500000001</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="3">
         <v>49.40460358</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="3">
         <v>41.162783879999999</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="3">
         <v>33.868870680000001</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="3">
         <v>32.306303509999999</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="3">
         <v>28.331758700000002</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="3">
         <v>24.417023789999998</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="3">
         <v>27.10970571</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="3">
         <v>1</v>
       </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>95.932490502561805</v>
       </c>
@@ -9253,41 +10402,48 @@
         <v>4</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="5">
+      <c r="M5" s="3">
         <v>91.297891000000007</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="3">
         <v>80.178369459999999</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="3">
         <v>65.833162970000004</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="3">
         <v>56.797632569999998</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="3">
         <v>45.845515429999999</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="3">
         <v>37.163043889999997</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="3">
         <v>36.381683619999997</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="3">
         <v>33.134527660000003</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5" s="3">
         <v>29.891807570000001</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="3">
         <v>26.11948469</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5" s="3">
         <v>3</v>
       </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>78.167438297246306</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>95.720350083546194</v>
       </c>
@@ -9322,41 +10478,48 @@
         <v>7</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>91.469560580000007</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>80.47497869</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="3">
         <v>67.884875230000006</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="3">
         <v>49.267962789999999</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="3">
         <v>44.49094316</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="3">
         <v>40.805040320000003</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="3">
         <v>40.507020689999997</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="3">
         <v>30.023509019999999</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="3">
         <v>26.474522799999999</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="3">
         <v>26.049409969999999</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="3">
         <v>6</v>
       </c>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>78.101908455161194</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>96.422198914457795</v>
       </c>
@@ -9391,70 +10554,84 @@
         <v>10</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="5">
+      <c r="M7" s="3">
         <v>92.267081430000005</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>78.493925110000006</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="3">
         <v>61.151521590000002</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="3">
         <v>53.399997650000003</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="3">
         <v>44.598546679999998</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="3">
         <v>40.269158240000003</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="3">
         <v>33.613865490000002</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="3">
         <v>29.000524599999999</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="3">
         <v>33.224392649999999</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="3">
         <v>21.85102646</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="3">
         <v>8</v>
       </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="3">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>71.223060238746299</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="3">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>77.3872378120288</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -9522,288 +10699,309 @@
       <c r="W9" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="3">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>83.941246715456401</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>95.564177950000001</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>78.128024870000004</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>55.64181044</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>40.420796559999999</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>40.783469570000001</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>39.470371579999998</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>28.98993402</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>35.432998750000003</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>29.83029531</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <v>31.896307539999999</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="3">
         <v>1</v>
       </c>
       <c r="L10" s="2"/>
-      <c r="M10" s="5">
+      <c r="M10" s="3">
         <v>89.860501319999997</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="3">
         <v>82.655543199999997</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="3">
         <v>61.226753500000001</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="3">
         <v>49.40460358</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="3">
         <v>41.162783879999999</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="3">
         <v>33.868870680000001</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S10" s="3">
         <v>32.306303509999999</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="3">
         <v>28.331758700000002</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10" s="3">
         <v>24.417023789999998</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10" s="3">
         <v>27.10970571</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="3">
         <v>1</v>
       </c>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="3">
+        <v>12</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>85.080659584638397</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>95.045101560000006</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>69.566130380000004</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>50.863828069999997</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>44.389371240000003</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>41.580493330000003</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>35.12641473</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <v>32.322934670000002</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>34.395285909999998</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="3">
         <v>32.646208770000001</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
         <v>29.357472609999999</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="3">
         <v>4</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="5">
+      <c r="M11" s="3">
         <v>91.297891000000007</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="3">
         <v>80.185471010000001</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="3">
         <v>67.75903941</v>
       </c>
-      <c r="P11" s="5">
+      <c r="P11" s="3">
         <v>57.333171739999997</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="3">
         <v>45.779895529999997</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="3">
         <v>37.696328299999998</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S11" s="3">
         <v>33.475340180000003</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="3">
         <v>30.806774229999998</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="3">
         <v>29.402273470000001</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="3">
         <v>25.328478990000001</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11" s="3">
         <v>3</v>
       </c>
+      <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>95.720350080000003</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>75.577600910000001</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>48.569220569999999</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>37.462311560000003</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>38.900668969999998</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>37.387228729999997</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <v>42.284651369999999</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <v>32.470959039999997</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="3">
         <v>30.876627419999998</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <v>32.585722250000003</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="3">
         <v>7</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="5">
+      <c r="M12" s="3">
         <v>92.391686719999996</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="3">
         <v>76.531750470000006</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="3">
         <v>64.044252599999993</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="3">
         <v>47.69022227</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="3">
         <v>43.0539858</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="3">
         <v>36.289046859999999</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="3">
         <v>37.63556122</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T12" s="3">
         <v>27.547677239999999</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="3">
         <v>25.812370380000001</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="3">
         <v>26.552556410000001</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="3">
         <v>6</v>
       </c>
+      <c r="X12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>95.998399250000006</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>68.063786559999997</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>49.08991821</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>41.897991959999999</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>35.163451019999997</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>33.052237359999999</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <v>32.132500440000001</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="3">
         <v>27.681891369999999</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="3">
         <v>32.624900250000003</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>32.038074020000003</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="3">
         <v>10</v>
       </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="5">
+      <c r="M13" s="3">
         <v>92.973048439999999</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="3">
         <v>76.325017360000004</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="3">
         <v>58.901209889999997</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="3">
         <v>52.027769110000001</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13" s="3">
         <v>42.708288179999997</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="3">
         <v>38.775578529999997</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="3">
         <v>33.449167520000003</v>
       </c>
-      <c r="T13" s="5">
+      <c r="T13" s="3">
         <v>30.35771149</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="3">
         <v>32.664232910000003</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="3">
         <v>21.176051430000001</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="3">
         <v>8</v>
       </c>
+      <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="L14" s="2"/>
+      <c r="X14" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="Y1:AH1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Y3:AI3"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="M8:W8"/>
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
new data and graphs
</commit_message>
<xml_diff>
--- a/proj1/report/data.xlsx
+++ b/proj1/report/data.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="440" windowWidth="18060" windowHeight="14020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="our_accuracy" localSheetId="0">Sheet1!$A$3:$K$7</definedName>
-    <definedName name="our_accuracy_animals" localSheetId="0">Sheet1!$M$3:$W$7</definedName>
-    <definedName name="our_accuracy_wine_2_relevant_1" localSheetId="0">Sheet1!$AA$5:$AK$8</definedName>
-    <definedName name="scikit_accuracy" localSheetId="0">Sheet1!$A$10:$K$15</definedName>
+    <definedName name="our_accuracy_animals_1" localSheetId="0">Sheet1!$M$3:$W$8</definedName>
+    <definedName name="our_accuracy_iris_1" localSheetId="0">Sheet1!$A$3:$K$8</definedName>
+    <definedName name="scikit_accuracy_animals" localSheetId="0">Sheet1!$M$10:$W$15</definedName>
+    <definedName name="scikit_accuracy_iris" localSheetId="0">Sheet1!$A$10:$K$15</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -68,8 +68,22 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="our_accuracy-wine-2-relevant" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="3" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/our_accuracy-wine-2-relevant.csv" comma="1">
+  <connection id="3" name="our_accuracy-animals1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/our_accuracy-animals.csv" comma="1">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="our_accuracy-iris" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/our_accuracy-iris.csv" comma="1">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="our_accuracy-wine-2-relevant" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="3" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/our_accuracy-wine-2-relevant.csv" comma="1">
       <textFields count="11">
         <textField/>
         <textField/>
@@ -85,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="scikit_accuracy" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="scikit_accuracy" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Jerry/Documents/thick-filling/proj1/code/scikit_accuracy.csv" tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -102,11 +116,25 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="7" name="scikit_accuracy-animals" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/scikit_accuracy-animals.csv" comma="1">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="scikit_accuracy-iris" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Gururaj/Documents/Senior Year/Fall Semester/Machine Learning/Project1/thick-filling/proj1/report/scikit_accuracy-iris.csv" comma="1">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>IRIS DATASET PERFORMANCE</t>
   </si>
@@ -133,6 +161,9 @@
   </si>
   <si>
     <t>Average Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> K-NN</t>
   </si>
 </sst>
 </file>
@@ -212,13 +243,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -278,9 +309,37 @@
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Accuracy of Our K-NN Classifier on the Iris Dataset</a:t>
+              <a:t>Accuracy of Our K-NN Classifier on the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>🌸</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dataset </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(many k)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -388,34 +447,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.5641779525474</c:v>
+                  <c:v>95.87638796654331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.12802487443621</c:v>
+                  <c:v>80.12333480907969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.6418104429592</c:v>
+                  <c:v>53.9832003028688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.4207965598681</c:v>
+                  <c:v>35.5736275542918</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.7834695673586</c:v>
+                  <c:v>36.3983340241275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.4703715841231</c:v>
+                  <c:v>33.7474283158975</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.9899340199751</c:v>
+                  <c:v>31.8723055869886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.4329987526313</c:v>
+                  <c:v>36.2779409326725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.830295305146</c:v>
+                  <c:v>32.6901685286616</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.8963075445477</c:v>
+                  <c:v>33.2895835379627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,7 +485,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>4-NN</c:v>
+            <c:v>3-NN</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="44450" cap="rnd">
@@ -489,34 +548,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.93249050256181</c:v>
+                  <c:v>96.3796919660262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.2775636204162</c:v>
+                  <c:v>75.05714209454349</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.4280021597867</c:v>
+                  <c:v>46.6391951398397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.7539236783358</c:v>
+                  <c:v>40.3552198563671</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.02347299194</c:v>
+                  <c:v>40.2870697258186</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.6181842350693</c:v>
+                  <c:v>37.0424014066685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.8278054581953</c:v>
+                  <c:v>32.9347787369649</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.2065215713908</c:v>
+                  <c:v>33.8364648410902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.1685941906401</c:v>
+                  <c:v>33.5564652777476</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.6081051071799</c:v>
+                  <c:v>27.2437896560835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,7 +586,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>7-NN</c:v>
+            <c:v>5-NN</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="44450" cap="rnd">
@@ -590,34 +649,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.72035008354619</c:v>
+                  <c:v>96.0382976369969</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75.8907680635923</c:v>
+                  <c:v>75.9141063150809</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.9441615979932</c:v>
+                  <c:v>54.3440600550579</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.5333320386658</c:v>
+                  <c:v>40.8007149926737</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.7467281840924</c:v>
+                  <c:v>40.7283399280904</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.1268671669177</c:v>
+                  <c:v>39.0314352844076</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.8950525882044</c:v>
+                  <c:v>38.0369526513788</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.6872567196358</c:v>
+                  <c:v>34.9508499227344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.0088846476567</c:v>
+                  <c:v>29.4849624489105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.5824195881053</c:v>
+                  <c:v>31.6488213322474</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -628,7 +687,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>10-NN</c:v>
+            <c:v>7-NN</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="47625" cap="rnd">
@@ -688,34 +747,134 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>96.42219891445779</c:v>
+                  <c:v>96.0218199248761</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.0500906577837</c:v>
+                  <c:v>72.71637989532969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.4669146264906</c:v>
+                  <c:v>54.1383511346862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.2939845537271</c:v>
+                  <c:v>47.4412956040492</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.0449753636994</c:v>
+                  <c:v>37.6799822830487</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.6035980045208</c:v>
+                  <c:v>32.0853264487581</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.9337701353752</c:v>
+                  <c:v>35.2201095461031</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.8568223411493</c:v>
+                  <c:v>31.5781861732618</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.7653103216837</c:v>
+                  <c:v>30.4167339699529</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.6213851591108</c:v>
+                  <c:v>34.625170620172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>9-NN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="53000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>96.3142361975727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.3826767018934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.678301360993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.9778941630234</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0845632674845</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.2995771167936</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.3942361089498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.8146256726098</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.1159415136391</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0539459443346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,11 +889,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1108098976"/>
-        <c:axId val="-1150582464"/>
+        <c:axId val="-464039424"/>
+        <c:axId val="-464036032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1108098976"/>
+        <c:axId val="-464039424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -846,12 +1005,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150582464"/>
+        <c:crossAx val="-464036032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1150582464"/>
+        <c:axId val="-464036032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -963,7 +1122,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1108098976"/>
+        <c:crossAx val="-464039424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1083,7 +1242,21 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of 1-NN vs 7-NN Using Our K-NN Classifier on the Iris Dataset</a:t>
+              <a:t> of 1-NN vs 7-NN Using Our K-NN Classifier on the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>🌸</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Dataset</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1184,39 +1357,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$6:$J$6</c:f>
+              <c:f>Sheet1!$A$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.72035008354619</c:v>
+                  <c:v>96.0218199248761</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75.8907680635923</c:v>
+                  <c:v>72.71637989532969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.9441615979932</c:v>
+                  <c:v>54.1383511346862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.5333320386658</c:v>
+                  <c:v>47.4412956040492</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.7467281840924</c:v>
+                  <c:v>37.6799822830487</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.1268671669177</c:v>
+                  <c:v>32.0853264487581</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.8950525882044</c:v>
+                  <c:v>35.2201095461031</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.6872567196358</c:v>
+                  <c:v>31.5781861732618</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.0088846476567</c:v>
+                  <c:v>30.4167339699529</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.5824195881053</c:v>
+                  <c:v>34.625170620172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1289,34 +1462,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.5641779525474</c:v>
+                  <c:v>95.87638796654331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.12802487443621</c:v>
+                  <c:v>80.12333480907969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.6418104429592</c:v>
+                  <c:v>53.9832003028688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.4207965598681</c:v>
+                  <c:v>35.5736275542918</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.7834695673586</c:v>
+                  <c:v>36.3983340241275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.4703715841231</c:v>
+                  <c:v>33.7474283158975</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.9899340199751</c:v>
+                  <c:v>31.8723055869886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.4329987526313</c:v>
+                  <c:v>36.2779409326725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.830295305146</c:v>
+                  <c:v>32.6901685286616</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.8963075445477</c:v>
+                  <c:v>33.2895835379627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,11 +1504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1072612144"/>
-        <c:axId val="-1072608752"/>
+        <c:axId val="-464005616"/>
+        <c:axId val="-464002224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1072612144"/>
+        <c:axId val="-464005616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -1440,12 +1613,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072608752"/>
+        <c:crossAx val="-464002224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1072608752"/>
+        <c:axId val="-464002224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1557,7 +1730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072612144"/>
+        <c:crossAx val="-464005616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1673,8 +1846,27 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>4-NN Classifier</a:t>
+              <a:t>3-NN Classifier</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> on the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>🌸</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Dataset</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1780,34 +1972,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.93249050256181</c:v>
+                  <c:v>96.3796919660262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.2775636204162</c:v>
+                  <c:v>75.05714209454349</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.4280021597867</c:v>
+                  <c:v>46.6391951398397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.7539236783358</c:v>
+                  <c:v>40.3552198563671</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.02347299194</c:v>
+                  <c:v>40.2870697258186</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.6181842350693</c:v>
+                  <c:v>37.0424014066685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.8278054581953</c:v>
+                  <c:v>32.9347787369649</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.2065215713908</c:v>
+                  <c:v>33.8364648410902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.1685941906401</c:v>
+                  <c:v>33.5564652777476</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.6081051071799</c:v>
+                  <c:v>27.2437896560835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1834,7 +2026,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$J$9</c:f>
+              <c:f>Sheet1!$A$10:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1873,39 +2065,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$11:$J$11</c:f>
+              <c:f>Sheet1!$A$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.04510156</c:v>
+                  <c:v>96.3796919660262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.56613038</c:v>
+                  <c:v>74.7120608095703</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.86382807</c:v>
+                  <c:v>44.6125657820502</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.38937124</c:v>
+                  <c:v>40.9516927103312</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.58049333</c:v>
+                  <c:v>38.9061571118433</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.12641473</c:v>
+                  <c:v>36.6716030113923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.32293467</c:v>
+                  <c:v>32.2527266708003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.39528591</c:v>
+                  <c:v>33.9302413045926</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.64620877</c:v>
+                  <c:v>32.3989276538469</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.35747261</c:v>
+                  <c:v>26.6863905571096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1920,11 +2112,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1072577840"/>
-        <c:axId val="-1072573808"/>
+        <c:axId val="-468389584"/>
+        <c:axId val="-468402000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1072577840"/>
+        <c:axId val="-468389584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -2029,12 +2221,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072573808"/>
+        <c:crossAx val="-468402000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1072573808"/>
+        <c:axId val="-468402000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2147,7 +2339,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072577840"/>
+        <c:crossAx val="-468389584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2263,8 +2455,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>1-NN Classifier</a:t>
+              <a:t>1-NN Classifier </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>on the Iris Dataset</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2324,7 +2527,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$J$9</c:f>
+              <c:f>Sheet1!$A$10:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2368,34 +2571,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.5641779525474</c:v>
+                  <c:v>95.87638796654331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.12802487443621</c:v>
+                  <c:v>80.12333480907969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.6418104429592</c:v>
+                  <c:v>53.9832003028688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.4207965598681</c:v>
+                  <c:v>35.5736275542918</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.7834695673586</c:v>
+                  <c:v>36.3983340241275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.4703715841231</c:v>
+                  <c:v>33.7474283158975</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.9899340199751</c:v>
+                  <c:v>31.8723055869886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.4329987526313</c:v>
+                  <c:v>36.2779409326725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.830295305146</c:v>
+                  <c:v>32.6901685286616</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.8963075445477</c:v>
+                  <c:v>33.2895835379627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2423,7 +2626,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$J$9</c:f>
+              <c:f>Sheet1!$A$10:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2462,39 +2665,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$J$10</c:f>
+              <c:f>Sheet1!$A$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.56417795</c:v>
+                  <c:v>95.87638796654331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.12802487</c:v>
+                  <c:v>80.12333480907969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.64181044</c:v>
+                  <c:v>53.9832003028688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.42079656</c:v>
+                  <c:v>35.5736275542918</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.78346957</c:v>
+                  <c:v>36.3983340241275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.47037158</c:v>
+                  <c:v>33.7474283158975</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.98993402</c:v>
+                  <c:v>31.8723055869886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.43299875</c:v>
+                  <c:v>36.2779409326725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.83029531</c:v>
+                  <c:v>32.6901685286616</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.89630754</c:v>
+                  <c:v>33.2895835379627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2509,11 +2712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1072547232"/>
-        <c:axId val="-1072543200"/>
+        <c:axId val="-463905280"/>
+        <c:axId val="-463901248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1072547232"/>
+        <c:axId val="-463905280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -2617,12 +2820,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072543200"/>
+        <c:crossAx val="-463901248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1072543200"/>
+        <c:axId val="-463901248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2735,7 +2938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072547232"/>
+        <c:crossAx val="-463905280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2956,34 +3159,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.5641779525474</c:v>
+                  <c:v>95.87638796654331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.12802487443621</c:v>
+                  <c:v>80.12333480907969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.6418104429592</c:v>
+                  <c:v>53.9832003028688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.4207965598681</c:v>
+                  <c:v>35.5736275542918</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.7834695673586</c:v>
+                  <c:v>36.3983340241275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.4703715841231</c:v>
+                  <c:v>33.7474283158975</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.9899340199751</c:v>
+                  <c:v>31.8723055869886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.4329987526313</c:v>
+                  <c:v>36.2779409326725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.830295305146</c:v>
+                  <c:v>32.6901685286616</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.8963075445477</c:v>
+                  <c:v>33.2895835379627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3054,34 +3257,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>89.86050132</c:v>
+                  <c:v>89.8351716592081</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.6555432</c:v>
+                  <c:v>80.7149630136681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.2267535</c:v>
+                  <c:v>61.8121197496832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.40460358</c:v>
+                  <c:v>47.1224097697605</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.16278388</c:v>
+                  <c:v>46.2855044395683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.86887068</c:v>
+                  <c:v>30.0320032309777</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.30630351</c:v>
+                  <c:v>29.0449184868868</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.3317587</c:v>
+                  <c:v>27.9270882836373</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.41702379</c:v>
+                  <c:v>21.685182416223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.10970571</c:v>
+                  <c:v>29.0287964371846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3096,11 +3299,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1072525296"/>
-        <c:axId val="-1072521264"/>
+        <c:axId val="-492212848"/>
+        <c:axId val="-492208736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1072525296"/>
+        <c:axId val="-492212848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -3212,12 +3415,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072521264"/>
+        <c:crossAx val="-492208736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1072521264"/>
+        <c:axId val="-492208736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3329,7 +3532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072525296"/>
+        <c:crossAx val="-492212848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3343,16 +3546,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.928909037210124"/>
-          <c:y val="0.393008756205079"/>
-          <c:w val="0.0710909627898762"/>
-          <c:h val="0.188930724261401"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3461,7 +3655,21 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of 1-NN vs 7-NN Using Our K-NN Classifier on the AnimalsDataset</a:t>
+              <a:t> of 1-NN vs 7-NN Using Our K-NN Classifier on the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>🐰</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Dataset</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3562,39 +3770,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$6:$V$6</c:f>
+              <c:f>Sheet1!$M$7:$V$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>91.46956058</c:v>
+                  <c:v>92.9367137470716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.47497869</c:v>
+                  <c:v>75.35372827627209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.88487523000001</c:v>
+                  <c:v>63.3877000789416</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.26796279</c:v>
+                  <c:v>53.7925958545981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.49094316</c:v>
+                  <c:v>44.7220781228465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.80504032</c:v>
+                  <c:v>41.4386660720621</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.50702069</c:v>
+                  <c:v>32.1914034802555</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.02350902</c:v>
+                  <c:v>26.5329342306431</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.4745228</c:v>
+                  <c:v>29.4602509765902</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.04940997</c:v>
+                  <c:v>25.3704799843921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3665,34 +3873,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>89.86050132</c:v>
+                  <c:v>89.8351716592081</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.6555432</c:v>
+                  <c:v>80.7149630136681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.2267535</c:v>
+                  <c:v>61.8121197496832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.40460358</c:v>
+                  <c:v>47.1224097697605</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.16278388</c:v>
+                  <c:v>46.2855044395683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.86887068</c:v>
+                  <c:v>30.0320032309777</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.30630351</c:v>
+                  <c:v>29.0449184868868</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.3317587</c:v>
+                  <c:v>27.9270882836373</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.41702379</c:v>
+                  <c:v>21.685182416223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.10970571</c:v>
+                  <c:v>29.0287964371846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3707,11 +3915,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1072491856"/>
-        <c:axId val="-1072487824"/>
+        <c:axId val="-465433648"/>
+        <c:axId val="-465400736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1072491856"/>
+        <c:axId val="-465433648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -3816,12 +4024,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072487824"/>
+        <c:crossAx val="-465400736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1072487824"/>
+        <c:axId val="-465400736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3903,6 +4111,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3933,7 +4142,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1072491856"/>
+        <c:crossAx val="-465433648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4051,9 +4260,37 @@
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Accuracy of Our K-NN Classifier on the Animals Dataset</a:t>
+              <a:t>Accuracy of Our K-NN Classifier on the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>🐰</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dataset </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(many k)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -4115,7 +4352,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$J$3</c:f>
+              <c:f>Sheet1!$M$3:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4159,34 +4396,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>89.86050132</c:v>
+                  <c:v>89.8351716592081</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.6555432</c:v>
+                  <c:v>80.7149630136681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.2267535</c:v>
+                  <c:v>61.8121197496832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.40460358</c:v>
+                  <c:v>47.1224097697605</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.16278388</c:v>
+                  <c:v>46.2855044395683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.86887068</c:v>
+                  <c:v>30.0320032309777</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.30630351</c:v>
+                  <c:v>29.0449184868868</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.3317587</c:v>
+                  <c:v>27.9270882836373</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.41702379</c:v>
+                  <c:v>21.685182416223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.10970571</c:v>
+                  <c:v>29.0287964371846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4197,7 +4434,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>4-NN</c:v>
+            <c:v>3-NN</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4213,7 +4450,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$J$3</c:f>
+              <c:f>Sheet1!$M$3:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4257,34 +4494,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>91.297891</c:v>
+                  <c:v>91.565626380756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.17836946</c:v>
+                  <c:v>80.6840242603875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.83316297</c:v>
+                  <c:v>64.8640882427018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.79763257</c:v>
+                  <c:v>53.3746931278354</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.84551543</c:v>
+                  <c:v>42.5831159849583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.16304389</c:v>
+                  <c:v>33.455956397993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.38168362</c:v>
+                  <c:v>30.240632114369</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.13452766</c:v>
+                  <c:v>29.6997262549017</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.89180757</c:v>
+                  <c:v>25.6763037641376</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.11948469</c:v>
+                  <c:v>20.1499231485486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4295,7 +4532,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>7-NN</c:v>
+            <c:v>5-NN</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4311,7 +4548,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$J$3</c:f>
+              <c:f>Sheet1!$M$3:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4355,34 +4592,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>91.46956058</c:v>
+                  <c:v>91.907926636556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.47497869</c:v>
+                  <c:v>76.5698967163658</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.88487523000001</c:v>
+                  <c:v>64.9330841434867</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.26796279</c:v>
+                  <c:v>46.7948251324264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.49094316</c:v>
+                  <c:v>43.1095607542829</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.80504032</c:v>
+                  <c:v>39.5464308513273</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.50702069</c:v>
+                  <c:v>36.9425019634787</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.02350902</c:v>
+                  <c:v>30.4673107335943</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.4745228</c:v>
+                  <c:v>26.3185343876274</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.04940997</c:v>
+                  <c:v>27.6964817372563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4393,7 +4630,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>10-NN</c:v>
+            <c:v>7-NN</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4409,7 +4646,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$J$3</c:f>
+              <c:f>Sheet1!$M$3:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4453,34 +4690,132 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>92.26708143</c:v>
+                  <c:v>92.9367137470716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.49392511</c:v>
+                  <c:v>75.35372827627209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.15152159</c:v>
+                  <c:v>63.3877000789416</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.39999765</c:v>
+                  <c:v>53.7925958545981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.59854668</c:v>
+                  <c:v>44.7220781228465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.26915824</c:v>
+                  <c:v>41.4386660720621</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.61386549</c:v>
+                  <c:v>32.1914034802555</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.0005246</c:v>
+                  <c:v>26.5329342306431</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.22439265</c:v>
+                  <c:v>29.4602509765902</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.85102646</c:v>
+                  <c:v>25.3704799843921</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>9-NN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$V$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$8:$V$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>93.09108225953049</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.23928727892461</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.2801651867539</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.8483428201041</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.671104683091</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.1123327143856</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.5202117167764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.3570947657834</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.1596207093873</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.4165092172522</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4495,11 +4830,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1108054320"/>
-        <c:axId val="-1108049776"/>
+        <c:axId val="-463876752"/>
+        <c:axId val="-463872720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1108054320"/>
+        <c:axId val="-463876752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -4611,12 +4946,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1108049776"/>
+        <c:crossAx val="-463872720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1108049776"/>
+        <c:axId val="-463872720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -4728,7 +5063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1108054320"/>
+        <c:crossAx val="-463876752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4856,7 +5191,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4972,11 +5306,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1013327136"/>
-        <c:axId val="-1014940752"/>
+        <c:axId val="-465250272"/>
+        <c:axId val="-465177008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1013327136"/>
+        <c:axId val="-465250272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5027,7 +5361,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5094,7 +5427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1014940752"/>
+        <c:crossAx val="-465177008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5102,7 +5435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1014940752"/>
+        <c:axId val="-465177008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5148,7 +5481,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5214,7 +5546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1013327136"/>
+        <c:crossAx val="-465250272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9578,13 +9910,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>425215</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>58795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>211667</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>136641</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9608,13 +9940,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>453203</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>191911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>878417</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>2586</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9638,13 +9970,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>505648</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>70556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>388055</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>188146</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9670,13 +10002,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>482130</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>58797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>81845</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>61149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9702,13 +10034,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>348075</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>117592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>352779</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>188147</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9732,13 +10064,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>223427</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>625122</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>10583</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9764,13 +10096,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>599724</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>47036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>303861</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>124883</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9794,16 +10126,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>489185</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>110066</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>712612</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>98306</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>82314</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>82314</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>305740</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>70554</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9826,25 +10158,25 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy-wine-2-relevant_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy-animals_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy-animals" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scikit_accuracy-animals" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scikit_accuracy" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy-iris_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="our_accuracy" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scikit_accuracy-iris" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Red Orange">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9852,34 +10184,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="505046"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="E84C22"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="FFBD47"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="B64926"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="FF8427"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="CC9900"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="B22600"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="CC9900"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="666699"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -10104,18 +10436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI14"/>
+  <dimension ref="A1:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="108" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="1" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
     <col min="13" max="22" width="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.5" customWidth="1"/>
+    <col min="23" max="23" width="5.5" customWidth="1"/>
     <col min="25" max="25" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
     <col min="27" max="34" width="13" bestFit="1" customWidth="1"/>
@@ -10125,88 +10457,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
       <c r="X1" s="2"/>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -10240,7 +10572,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="1">
@@ -10274,87 +10606,87 @@
         <v>18</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="X3" s="2"/>
-      <c r="Y3" s="4" t="s">
+      <c r="Y3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>95.564177952547396</v>
+        <v>95.876387966543305</v>
       </c>
       <c r="B4">
-        <v>78.128024874436207</v>
+        <v>80.123334809079694</v>
       </c>
       <c r="C4">
-        <v>55.641810442959198</v>
+        <v>53.983200302868802</v>
       </c>
       <c r="D4">
-        <v>40.420796559868101</v>
+        <v>35.573627554291797</v>
       </c>
       <c r="E4">
-        <v>40.783469567358601</v>
+        <v>36.3983340241275</v>
       </c>
       <c r="F4">
-        <v>39.4703715841231</v>
+        <v>33.747428315897501</v>
       </c>
       <c r="G4">
-        <v>28.989934019975099</v>
+        <v>31.872305586988599</v>
       </c>
       <c r="H4">
-        <v>35.432998752631299</v>
+        <v>36.2779409326725</v>
       </c>
       <c r="I4">
-        <v>29.830295305145999</v>
+        <v>32.690168528661601</v>
       </c>
       <c r="J4">
-        <v>31.8963075445477</v>
+        <v>33.289583537962699</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="3">
-        <v>89.860501319999997</v>
+        <v>89.8351716592081</v>
       </c>
       <c r="N4" s="3">
-        <v>82.655543199999997</v>
+        <v>80.714963013668097</v>
       </c>
       <c r="O4" s="3">
-        <v>61.226753500000001</v>
+        <v>61.812119749683198</v>
       </c>
       <c r="P4" s="3">
-        <v>49.40460358</v>
+        <v>47.122409769760502</v>
       </c>
       <c r="Q4" s="3">
-        <v>41.162783879999999</v>
+        <v>46.2855044395683</v>
       </c>
       <c r="R4" s="3">
-        <v>33.868870680000001</v>
+        <v>30.032003230977701</v>
       </c>
       <c r="S4" s="3">
-        <v>32.306303509999999</v>
+        <v>29.0449184868868</v>
       </c>
       <c r="T4" s="3">
-        <v>28.331758700000002</v>
+        <v>27.9270882836373</v>
       </c>
       <c r="U4" s="3">
-        <v>24.417023789999998</v>
+        <v>21.685182416223</v>
       </c>
       <c r="V4" s="3">
-        <v>27.10970571</v>
+        <v>29.028796437184599</v>
       </c>
       <c r="W4" s="3">
         <v>1</v>
@@ -10369,68 +10701,68 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>95.932490502561805</v>
+        <v>96.379691966026201</v>
       </c>
       <c r="B5">
-        <v>71.277563620416203</v>
+        <v>75.057142094543494</v>
       </c>
       <c r="C5">
-        <v>52.428002159786701</v>
+        <v>46.6391951398397</v>
       </c>
       <c r="D5">
-        <v>44.753923678335802</v>
+        <v>40.3552198563671</v>
       </c>
       <c r="E5">
-        <v>42.023472991939997</v>
+        <v>40.287069725818597</v>
       </c>
       <c r="F5">
-        <v>32.6181842350693</v>
+        <v>37.042401406668503</v>
       </c>
       <c r="G5">
-        <v>31.8278054581953</v>
+        <v>32.934778736964901</v>
       </c>
       <c r="H5">
-        <v>35.206521571390802</v>
+        <v>33.836464841090198</v>
       </c>
       <c r="I5">
-        <v>34.1685941906401</v>
+        <v>33.556465277747598</v>
       </c>
       <c r="J5">
-        <v>29.608105107179899</v>
+        <v>27.2437896560835</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="3">
-        <v>91.297891000000007</v>
+        <v>91.565626380756001</v>
       </c>
       <c r="N5" s="3">
-        <v>80.178369459999999</v>
+        <v>80.684024260387503</v>
       </c>
       <c r="O5" s="3">
-        <v>65.833162970000004</v>
+        <v>64.864088242701797</v>
       </c>
       <c r="P5" s="3">
-        <v>56.797632569999998</v>
+        <v>53.3746931278354</v>
       </c>
       <c r="Q5" s="3">
-        <v>45.845515429999999</v>
+        <v>42.583115984958297</v>
       </c>
       <c r="R5" s="3">
-        <v>37.163043889999997</v>
+        <v>33.455956397992999</v>
       </c>
       <c r="S5" s="3">
-        <v>36.381683619999997</v>
+        <v>30.240632114368999</v>
       </c>
       <c r="T5" s="3">
-        <v>33.134527660000003</v>
+        <v>29.699726254901702</v>
       </c>
       <c r="U5" s="3">
-        <v>29.891807570000001</v>
+        <v>25.6763037641376</v>
       </c>
       <c r="V5" s="3">
-        <v>26.11948469</v>
+        <v>20.149923148548599</v>
       </c>
       <c r="W5" s="3">
         <v>3</v>
@@ -10439,571 +10771,707 @@
       <c r="Y5" s="3">
         <v>2</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="Z5" s="4">
         <v>78.167438297246306</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>95.720350083546194</v>
+        <v>96.038297636996901</v>
       </c>
       <c r="B6">
-        <v>75.890768063592304</v>
+        <v>75.9141063150809</v>
       </c>
       <c r="C6">
-        <v>49.944161597993201</v>
+        <v>54.344060055057902</v>
       </c>
       <c r="D6">
-        <v>37.533332038665797</v>
+        <v>40.800714992673697</v>
       </c>
       <c r="E6">
-        <v>38.746728184092397</v>
+        <v>40.728339928090399</v>
       </c>
       <c r="F6">
-        <v>37.126867166917698</v>
+        <v>39.0314352844076</v>
       </c>
       <c r="G6">
-        <v>42.8950525882044</v>
+        <v>38.036952651378797</v>
       </c>
       <c r="H6">
-        <v>32.687256719635798</v>
+        <v>34.950849922734399</v>
       </c>
       <c r="I6">
-        <v>30.0088846476567</v>
+        <v>29.484962448910501</v>
       </c>
       <c r="J6">
-        <v>32.582419588105303</v>
+        <v>31.648821332247401</v>
       </c>
       <c r="K6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="3">
-        <v>91.469560580000007</v>
+        <v>91.907926636555999</v>
       </c>
       <c r="N6" s="3">
-        <v>80.47497869</v>
+        <v>76.569896716365804</v>
       </c>
       <c r="O6" s="3">
-        <v>67.884875230000006</v>
+        <v>64.933084143486695</v>
       </c>
       <c r="P6" s="3">
-        <v>49.267962789999999</v>
+        <v>46.794825132426404</v>
       </c>
       <c r="Q6" s="3">
-        <v>44.49094316</v>
+        <v>43.109560754282903</v>
       </c>
       <c r="R6" s="3">
-        <v>40.805040320000003</v>
+        <v>39.546430851327301</v>
       </c>
       <c r="S6" s="3">
-        <v>40.507020689999997</v>
+        <v>36.942501963478698</v>
       </c>
       <c r="T6" s="3">
-        <v>30.023509019999999</v>
+        <v>30.467310733594299</v>
       </c>
       <c r="U6" s="3">
-        <v>26.474522799999999</v>
+        <v>26.318534387627398</v>
       </c>
       <c r="V6" s="3">
-        <v>26.049409969999999</v>
+        <v>27.696481737256299</v>
       </c>
       <c r="W6" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="3">
         <v>4</v>
       </c>
-      <c r="Z6" s="6">
+      <c r="Z6" s="4">
         <v>78.101908455161194</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>96.422198914457795</v>
+        <v>96.021819924876098</v>
       </c>
       <c r="B7">
-        <v>72.050090657783699</v>
+        <v>72.716379895329695</v>
       </c>
       <c r="C7">
-        <v>49.466914626490599</v>
+        <v>54.138351134686197</v>
       </c>
       <c r="D7">
-        <v>42.2939845537271</v>
+        <v>47.441295604049202</v>
       </c>
       <c r="E7">
-        <v>34.0449753636994</v>
+        <v>37.679982283048702</v>
       </c>
       <c r="F7">
-        <v>32.603598004520798</v>
+        <v>32.085326448758103</v>
       </c>
       <c r="G7">
-        <v>32.933770135375198</v>
+        <v>35.220109546103103</v>
       </c>
       <c r="H7">
-        <v>26.8568223411493</v>
+        <v>31.578186173261798</v>
       </c>
       <c r="I7">
-        <v>31.7653103216837</v>
+        <v>30.416733969952901</v>
       </c>
       <c r="J7">
-        <v>31.621385159110801</v>
+        <v>34.625170620172</v>
       </c>
       <c r="K7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="3">
-        <v>92.267081430000005</v>
+        <v>92.936713747071593</v>
       </c>
       <c r="N7" s="3">
-        <v>78.493925110000006</v>
+        <v>75.353728276272093</v>
       </c>
       <c r="O7" s="3">
-        <v>61.151521590000002</v>
+        <v>63.387700078941599</v>
       </c>
       <c r="P7" s="3">
-        <v>53.399997650000003</v>
+        <v>53.792595854598098</v>
       </c>
       <c r="Q7" s="3">
-        <v>44.598546679999998</v>
+        <v>44.722078122846497</v>
       </c>
       <c r="R7" s="3">
-        <v>40.269158240000003</v>
+        <v>41.438666072062098</v>
       </c>
       <c r="S7" s="3">
-        <v>33.613865490000002</v>
+        <v>32.191403480255502</v>
       </c>
       <c r="T7" s="3">
-        <v>29.000524599999999</v>
+        <v>26.5329342306431</v>
       </c>
       <c r="U7" s="3">
-        <v>33.224392649999999</v>
+        <v>29.460250976590199</v>
       </c>
       <c r="V7" s="3">
-        <v>21.85102646</v>
+        <v>25.370479984392102</v>
       </c>
       <c r="W7" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="3">
         <v>6</v>
       </c>
-      <c r="Z7" s="6">
+      <c r="Z7" s="4">
         <v>71.223060238746299</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="A8">
+        <v>96.314236197572697</v>
+      </c>
+      <c r="B8">
+        <v>69.382676701893402</v>
+      </c>
+      <c r="C8">
+        <v>48.678301360992997</v>
+      </c>
+      <c r="D8">
+        <v>42.9778941630234</v>
+      </c>
+      <c r="E8">
+        <v>40.084563267484498</v>
+      </c>
+      <c r="F8">
+        <v>34.2995771167936</v>
+      </c>
+      <c r="G8">
+        <v>31.394236108949801</v>
+      </c>
+      <c r="H8">
+        <v>35.8146256726098</v>
+      </c>
+      <c r="I8">
+        <v>40.1159415136391</v>
+      </c>
+      <c r="J8">
+        <v>32.0539459443346</v>
+      </c>
+      <c r="K8">
+        <v>9</v>
+      </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
+      <c r="M8" s="3">
+        <v>93.091082259530495</v>
+      </c>
+      <c r="N8" s="3">
+        <v>77.239287278924607</v>
+      </c>
+      <c r="O8" s="3">
+        <v>60.280165186753898</v>
+      </c>
+      <c r="P8" s="3">
+        <v>51.848342820104101</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>46.671104683091002</v>
+      </c>
+      <c r="R8" s="3">
+        <v>42.112332714385602</v>
+      </c>
+      <c r="S8" s="3">
+        <v>34.520211716776402</v>
+      </c>
+      <c r="T8" s="3">
+        <v>28.357094765783401</v>
+      </c>
+      <c r="U8" s="3">
+        <v>24.159620709387301</v>
+      </c>
+      <c r="V8" s="3">
+        <v>22.416509217252202</v>
+      </c>
+      <c r="W8" s="3">
+        <v>9</v>
+      </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="3">
         <v>8</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="Z8" s="4">
         <v>77.3872378120288</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1">
-        <v>14</v>
-      </c>
-      <c r="I9" s="1">
-        <v>16</v>
-      </c>
-      <c r="J9" s="1">
-        <v>18</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>2</v>
-      </c>
-      <c r="O9" s="1">
-        <v>4</v>
-      </c>
-      <c r="P9" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>8</v>
-      </c>
-      <c r="R9" s="1">
-        <v>10</v>
-      </c>
-      <c r="S9" s="1">
-        <v>12</v>
-      </c>
-      <c r="T9" s="1">
-        <v>14</v>
-      </c>
-      <c r="U9" s="1">
-        <v>16</v>
-      </c>
-      <c r="V9" s="1">
-        <v>18</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="M9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="3">
         <v>10</v>
       </c>
-      <c r="Z9" s="6">
+      <c r="Z9" s="4">
         <v>83.941246715456401</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>95.564177950000001</v>
-      </c>
-      <c r="B10" s="3">
-        <v>78.128024870000004</v>
-      </c>
-      <c r="C10" s="3">
-        <v>55.64181044</v>
-      </c>
-      <c r="D10" s="3">
-        <v>40.420796559999999</v>
-      </c>
-      <c r="E10" s="3">
-        <v>40.783469570000001</v>
-      </c>
-      <c r="F10" s="3">
-        <v>39.470371579999998</v>
-      </c>
-      <c r="G10" s="3">
-        <v>28.98993402</v>
-      </c>
-      <c r="H10" s="3">
-        <v>35.432998750000003</v>
-      </c>
-      <c r="I10" s="3">
-        <v>29.83029531</v>
-      </c>
-      <c r="J10" s="3">
-        <v>31.896307539999999</v>
-      </c>
-      <c r="K10" s="3">
-        <v>1</v>
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1">
+        <v>16</v>
+      </c>
+      <c r="J10" s="1">
+        <v>18</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="L10" s="2"/>
-      <c r="M10" s="3">
-        <v>89.860501319999997</v>
-      </c>
-      <c r="N10" s="3">
-        <v>82.655543199999997</v>
-      </c>
-      <c r="O10" s="3">
-        <v>61.226753500000001</v>
-      </c>
-      <c r="P10" s="3">
-        <v>49.40460358</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>41.162783879999999</v>
-      </c>
-      <c r="R10" s="3">
-        <v>33.868870680000001</v>
-      </c>
-      <c r="S10" s="3">
-        <v>32.306303509999999</v>
-      </c>
-      <c r="T10" s="3">
-        <v>28.331758700000002</v>
-      </c>
-      <c r="U10" s="3">
-        <v>24.417023789999998</v>
-      </c>
-      <c r="V10" s="3">
-        <v>27.10970571</v>
-      </c>
-      <c r="W10" s="3">
-        <v>1</v>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>4</v>
+      </c>
+      <c r="P10" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>8</v>
+      </c>
+      <c r="R10" s="1">
+        <v>10</v>
+      </c>
+      <c r="S10" s="1">
+        <v>12</v>
+      </c>
+      <c r="T10" s="1">
+        <v>14</v>
+      </c>
+      <c r="U10" s="1">
+        <v>16</v>
+      </c>
+      <c r="V10" s="1">
+        <v>18</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="3">
         <v>12</v>
       </c>
-      <c r="Z10" s="6">
+      <c r="Z10" s="4">
         <v>85.080659584638397</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>95.045101560000006</v>
+        <v>95.876387966543305</v>
       </c>
       <c r="B11" s="3">
-        <v>69.566130380000004</v>
+        <v>80.123334809079694</v>
       </c>
       <c r="C11" s="3">
-        <v>50.863828069999997</v>
+        <v>53.983200302868802</v>
       </c>
       <c r="D11" s="3">
-        <v>44.389371240000003</v>
+        <v>35.573627554291797</v>
       </c>
       <c r="E11" s="3">
-        <v>41.580493330000003</v>
+        <v>36.3983340241275</v>
       </c>
       <c r="F11" s="3">
-        <v>35.12641473</v>
+        <v>33.747428315897501</v>
       </c>
       <c r="G11" s="3">
-        <v>32.322934670000002</v>
+        <v>31.872305586988599</v>
       </c>
       <c r="H11" s="3">
-        <v>34.395285909999998</v>
+        <v>36.2779409326725</v>
       </c>
       <c r="I11" s="3">
-        <v>32.646208770000001</v>
+        <v>32.690168528661601</v>
       </c>
       <c r="J11" s="3">
-        <v>29.357472609999999</v>
+        <v>33.289583537962699</v>
       </c>
       <c r="K11" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="3">
-        <v>91.297891000000007</v>
+        <v>89.8351716592081</v>
       </c>
       <c r="N11" s="3">
-        <v>80.185471010000001</v>
+        <v>80.714963013668097</v>
       </c>
       <c r="O11" s="3">
-        <v>67.75903941</v>
+        <v>61.812119749683198</v>
       </c>
       <c r="P11" s="3">
-        <v>57.333171739999997</v>
+        <v>47.122409769760502</v>
       </c>
       <c r="Q11" s="3">
-        <v>45.779895529999997</v>
+        <v>46.2855044395683</v>
       </c>
       <c r="R11" s="3">
-        <v>37.696328299999998</v>
+        <v>30.032003230977701</v>
       </c>
       <c r="S11" s="3">
-        <v>33.475340180000003</v>
+        <v>29.0449184868868</v>
       </c>
       <c r="T11" s="3">
-        <v>30.806774229999998</v>
+        <v>27.9270882836373</v>
       </c>
       <c r="U11" s="3">
-        <v>29.402273470000001</v>
+        <v>21.685182416223</v>
       </c>
       <c r="V11" s="3">
-        <v>25.328478990000001</v>
+        <v>29.028796437184599</v>
       </c>
       <c r="W11" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>95.720350080000003</v>
+        <v>96.379691966026201</v>
       </c>
       <c r="B12" s="3">
-        <v>75.577600910000001</v>
+        <v>74.712060809570303</v>
       </c>
       <c r="C12" s="3">
-        <v>48.569220569999999</v>
+        <v>44.612565782050197</v>
       </c>
       <c r="D12" s="3">
-        <v>37.462311560000003</v>
+        <v>40.951692710331201</v>
       </c>
       <c r="E12" s="3">
-        <v>38.900668969999998</v>
+        <v>38.906157111843299</v>
       </c>
       <c r="F12" s="3">
-        <v>37.387228729999997</v>
+        <v>36.6716030113923</v>
       </c>
       <c r="G12" s="3">
-        <v>42.284651369999999</v>
+        <v>32.2527266708003</v>
       </c>
       <c r="H12" s="3">
-        <v>32.470959039999997</v>
+        <v>33.930241304592599</v>
       </c>
       <c r="I12" s="3">
-        <v>30.876627419999998</v>
+        <v>32.398927653846897</v>
       </c>
       <c r="J12" s="3">
-        <v>32.585722250000003</v>
+        <v>26.686390557109601</v>
       </c>
       <c r="K12" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="3">
-        <v>92.391686719999996</v>
+        <v>91.565626380756001</v>
       </c>
       <c r="N12" s="3">
-        <v>76.531750470000006</v>
+        <v>81.488132384852307</v>
       </c>
       <c r="O12" s="3">
-        <v>64.044252599999993</v>
+        <v>66.270611544253597</v>
       </c>
       <c r="P12" s="3">
-        <v>47.69022227</v>
+        <v>53.550618795971303</v>
       </c>
       <c r="Q12" s="3">
-        <v>43.0539858</v>
+        <v>42.854054587766903</v>
       </c>
       <c r="R12" s="3">
-        <v>36.289046859999999</v>
+        <v>31.475017731058799</v>
       </c>
       <c r="S12" s="3">
-        <v>37.63556122</v>
+        <v>29.688034095000301</v>
       </c>
       <c r="T12" s="3">
-        <v>27.547677239999999</v>
+        <v>28.0420389071434</v>
       </c>
       <c r="U12" s="3">
-        <v>25.812370380000001</v>
+        <v>26.1221835277404</v>
       </c>
       <c r="V12" s="3">
-        <v>26.552556410000001</v>
+        <v>20.557961555815901</v>
       </c>
       <c r="W12" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>95.998399250000006</v>
+        <v>96.038297636996901</v>
       </c>
       <c r="B13" s="3">
-        <v>68.063786559999997</v>
+        <v>76.409456154425499</v>
       </c>
       <c r="C13" s="3">
-        <v>49.08991821</v>
+        <v>57.067254428776899</v>
       </c>
       <c r="D13" s="3">
-        <v>41.897991959999999</v>
+        <v>41.968441093499401</v>
       </c>
       <c r="E13" s="3">
-        <v>35.163451019999997</v>
+        <v>41.849112124301598</v>
       </c>
       <c r="F13" s="3">
-        <v>33.052237359999999</v>
+        <v>38.329915080710897</v>
       </c>
       <c r="G13" s="3">
-        <v>32.132500440000001</v>
+        <v>39.108376138242797</v>
       </c>
       <c r="H13" s="3">
-        <v>27.681891369999999</v>
+        <v>35.2351394554153</v>
       </c>
       <c r="I13" s="3">
-        <v>32.624900250000003</v>
+        <v>29.914557740570501</v>
       </c>
       <c r="J13" s="3">
-        <v>32.038074020000003</v>
+        <v>32.644707921348797</v>
       </c>
       <c r="K13" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="3">
-        <v>92.973048439999999</v>
+        <v>91.907926636555999</v>
       </c>
       <c r="N13" s="3">
-        <v>76.325017360000004</v>
+        <v>77.445627850163405</v>
       </c>
       <c r="O13" s="3">
-        <v>58.901209889999997</v>
+        <v>65.6992584534418</v>
       </c>
       <c r="P13" s="3">
-        <v>52.027769110000001</v>
+        <v>46.864471679376102</v>
       </c>
       <c r="Q13" s="3">
-        <v>42.708288179999997</v>
+        <v>43.633889615439401</v>
       </c>
       <c r="R13" s="3">
-        <v>38.775578529999997</v>
+        <v>39.436746461276897</v>
       </c>
       <c r="S13" s="3">
-        <v>33.449167520000003</v>
+        <v>36.911138690478403</v>
       </c>
       <c r="T13" s="3">
-        <v>30.35771149</v>
+        <v>30.847827078233799</v>
       </c>
       <c r="U13" s="3">
-        <v>32.664232910000003</v>
+        <v>26.8407179590459</v>
       </c>
       <c r="V13" s="3">
-        <v>21.176051430000001</v>
+        <v>26.869183906216801</v>
       </c>
       <c r="W13" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>96.021819924876098</v>
+      </c>
+      <c r="B14" s="3">
+        <v>73.397477102195396</v>
+      </c>
+      <c r="C14" s="3">
+        <v>55.376235854048801</v>
+      </c>
+      <c r="D14" s="3">
+        <v>47.8847221111049</v>
+      </c>
+      <c r="E14" s="3">
+        <v>38.329862623197997</v>
+      </c>
+      <c r="F14" s="3">
+        <v>31.821341723813902</v>
+      </c>
+      <c r="G14" s="3">
+        <v>35.476697713732499</v>
+      </c>
+      <c r="H14" s="3">
+        <v>31.833886725978299</v>
+      </c>
+      <c r="I14" s="3">
+        <v>30.767201588784399</v>
+      </c>
+      <c r="J14" s="3">
+        <v>34.957615826285597</v>
+      </c>
+      <c r="K14" s="3">
+        <v>7</v>
+      </c>
       <c r="L14" s="2"/>
+      <c r="M14" s="3">
+        <v>92.936713747071593</v>
+      </c>
+      <c r="N14" s="3">
+        <v>75.021481582191399</v>
+      </c>
+      <c r="O14" s="3">
+        <v>63.489640587511403</v>
+      </c>
+      <c r="P14" s="3">
+        <v>54.482222456867497</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>44.055859404940698</v>
+      </c>
+      <c r="R14" s="3">
+        <v>41.268092033927999</v>
+      </c>
+      <c r="S14" s="3">
+        <v>31.794371926295199</v>
+      </c>
+      <c r="T14" s="3">
+        <v>25.865000161423499</v>
+      </c>
+      <c r="U14" s="3">
+        <v>28.359698891459001</v>
+      </c>
+      <c r="V14" s="3">
+        <v>25.1388904809404</v>
+      </c>
+      <c r="W14" s="3">
+        <v>7</v>
+      </c>
       <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>96.334236197572693</v>
+      </c>
+      <c r="B15">
+        <v>69.765350065054804</v>
+      </c>
+      <c r="C15">
+        <v>49.476290779718603</v>
+      </c>
+      <c r="D15">
+        <v>42.512738189416297</v>
+      </c>
+      <c r="E15">
+        <v>39.974945304968202</v>
+      </c>
+      <c r="F15">
+        <v>34.703425319044399</v>
+      </c>
+      <c r="G15">
+        <v>30.9190528523288</v>
+      </c>
+      <c r="H15">
+        <v>36.079958708118703</v>
+      </c>
+      <c r="I15">
+        <v>39.092386713616897</v>
+      </c>
+      <c r="J15">
+        <v>32.864650742806703</v>
+      </c>
+      <c r="K15">
+        <v>9</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15">
+        <v>93.091082259530495</v>
+      </c>
+      <c r="N15">
+        <v>77.475330140088502</v>
+      </c>
+      <c r="O15">
+        <v>60.595888308376701</v>
+      </c>
+      <c r="P15">
+        <v>52.681556900481198</v>
+      </c>
+      <c r="Q15">
+        <v>47.423337112853503</v>
+      </c>
+      <c r="R15">
+        <v>42.417847926317798</v>
+      </c>
+      <c r="S15">
+        <v>33.996287938073799</v>
+      </c>
+      <c r="T15">
+        <v>28.724829140032401</v>
+      </c>
+      <c r="U15">
+        <v>23.579895280548101</v>
+      </c>
+      <c r="V15">
+        <v>21.7881301742894</v>
+      </c>
+      <c r="W15">
+        <v>9</v>
+      </c>
+      <c r="X15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="Y1:AH1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Y3:AI3"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="M8:W8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="M9:W9"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:V1"/>
     <mergeCell ref="A2:K2"/>

</xml_diff>